<commit_message>
refactor: simplify test cases loading
</commit_message>
<xml_diff>
--- a/measurehero/tests/test_data/test_cases_fr.xlsx
+++ b/measurehero/tests/test_data/test_cases_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\File Filippo\Progetti\Python\Git Projects\Git_MeasureHero\measurehero\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD1934-0853-4633-8A9D-F083A1901101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE916DF-2125-4CBC-8FD1-6103E6AAFBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="3168" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>units</t>
   </si>
   <si>
-    <t>unitary_weight</t>
-  </si>
-  <si>
-    <t>total_weight</t>
-  </si>
-  <si>
     <t>unit_of_measure</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>mini gratin de choux fleurs 4x120g 480g</t>
+  </si>
+  <si>
+    <t>unitary_measure</t>
+  </si>
+  <si>
+    <t>total_measure</t>
   </si>
 </sst>
 </file>
@@ -430,13 +430,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -447,35 +448,32 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>250</v>
-      </c>
       <c r="D2">
         <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -483,16 +481,13 @@
       <c r="C3">
         <v>130</v>
       </c>
-      <c r="D3">
-        <v>260</v>
-      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -500,16 +495,13 @@
       <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -517,33 +509,27 @@
       <c r="C5">
         <v>200</v>
       </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>33.375</v>
-      </c>
       <c r="D6">
         <v>267</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -551,16 +537,13 @@
       <c r="C7">
         <v>60</v>
       </c>
-      <c r="D7">
-        <v>120</v>
-      </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>24</v>
@@ -568,58 +551,49 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>11.625</v>
-      </c>
       <c r="D9">
         <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>25</v>
       </c>
-      <c r="C10">
-        <v>1.6</v>
-      </c>
       <c r="D10">
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>0.88</v>
-      </c>
       <c r="D11">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -627,50 +601,41 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12">
-        <v>60</v>
-      </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>850</v>
-      </c>
       <c r="D13">
         <v>850</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>20</v>
-      </c>
       <c r="D14">
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -678,7 +643,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -686,16 +651,13 @@
       <c r="C16">
         <v>25</v>
       </c>
-      <c r="D16">
-        <v>150</v>
-      </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -703,16 +665,13 @@
       <c r="C17">
         <v>120</v>
       </c>
-      <c r="D17">
-        <v>480</v>
-      </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -720,11 +679,8 @@
       <c r="C18">
         <v>120</v>
       </c>
-      <c r="D18">
-        <v>240</v>
-      </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: logic to extract total measure
</commit_message>
<xml_diff>
--- a/measurehero/tests/test_data/test_cases_fr.xlsx
+++ b/measurehero/tests/test_data/test_cases_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\File Filippo\Progetti\Python\Git Projects\Git_MeasureHero\measurehero\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE916DF-2125-4CBC-8FD1-6103E6AAFBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD23CD-3244-4CA3-B20E-D57EBB2747B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,6 +665,9 @@
       <c r="C17">
         <v>120</v>
       </c>
+      <c r="D17">
+        <v>480</v>
+      </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
@@ -678,6 +681,9 @@
       </c>
       <c r="C18">
         <v>120</v>
+      </c>
+      <c r="D18">
+        <v>240</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
feat: include new pattern
</commit_message>
<xml_diff>
--- a/measurehero/tests/test_data/test_cases_fr.xlsx
+++ b/measurehero/tests/test_data/test_cases_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\File Filippo\Progetti\Python\Git Projects\Git_MeasureHero\measurehero\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD23CD-3244-4CA3-B20E-D57EBB2747B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F088112C-B1E5-4F7F-BABC-0E7ECE24CCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>input_string</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>total_measure</t>
+  </si>
+  <si>
+    <t>naturnes epinards des 4/6mois nestle bols 130g x 2</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +476,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -487,41 +490,41 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>267</v>
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -529,13 +532,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>60</v>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>267</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -543,35 +546,35 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>186</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>40</v>
+        <v>186</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -579,13 +582,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>25</v>
       </c>
       <c r="D11">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -593,99 +596,113 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>850</v>
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>850</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>120</v>
-      </c>
-      <c r="D17">
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>120</v>
       </c>
       <c r="D18">
+        <v>480</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>240</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: logic on a case base rather than on feature base
</commit_message>
<xml_diff>
--- a/measurehero/tests/test_data/test_cases_fr.xlsx
+++ b/measurehero/tests/test_data/test_cases_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\File Filippo\Progetti\Python\Git Projects\Git_MeasureHero\measurehero\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F088112C-B1E5-4F7F-BABC-0E7ECE24CCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56FF929-16A9-4018-A52A-05D311C16C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,6 +467,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
       <c r="D2">
         <v>250</v>
       </c>
@@ -484,6 +487,9 @@
       <c r="C3">
         <v>130</v>
       </c>
+      <c r="D3">
+        <v>260</v>
+      </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
@@ -498,6 +504,9 @@
       <c r="C4">
         <v>130</v>
       </c>
+      <c r="D4">
+        <v>260</v>
+      </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -512,6 +521,9 @@
       <c r="C5">
         <v>20</v>
       </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
@@ -526,6 +538,9 @@
       <c r="C6">
         <v>200</v>
       </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -537,6 +552,9 @@
       <c r="B7">
         <v>8</v>
       </c>
+      <c r="C7">
+        <v>33.375</v>
+      </c>
       <c r="D7">
         <v>267</v>
       </c>
@@ -554,6 +572,9 @@
       <c r="C8">
         <v>60</v>
       </c>
+      <c r="D8">
+        <v>120</v>
+      </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
@@ -573,6 +594,9 @@
       <c r="B10">
         <v>16</v>
       </c>
+      <c r="C10">
+        <v>11.625</v>
+      </c>
       <c r="D10">
         <v>186</v>
       </c>
@@ -587,6 +611,9 @@
       <c r="B11">
         <v>25</v>
       </c>
+      <c r="C11">
+        <v>1.6</v>
+      </c>
       <c r="D11">
         <v>40</v>
       </c>
@@ -601,6 +628,9 @@
       <c r="B12">
         <v>25</v>
       </c>
+      <c r="C12">
+        <v>0.88</v>
+      </c>
       <c r="D12">
         <v>22</v>
       </c>
@@ -618,6 +648,9 @@
       <c r="C13">
         <v>20</v>
       </c>
+      <c r="D13">
+        <v>60</v>
+      </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
@@ -629,6 +662,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>850</v>
+      </c>
       <c r="D14">
         <v>850</v>
       </c>
@@ -643,6 +679,9 @@
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
       <c r="D15">
         <v>20</v>
       </c>
@@ -667,6 +706,9 @@
       </c>
       <c r="C17">
         <v>25</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>

</xml_diff>